<commit_message>
Add presentation materials and some processed data
</commit_message>
<xml_diff>
--- a/resources/logs/20conv_30bs/Celeron_20conv_30bs.xlsx
+++ b/resources/logs/20conv_30bs/Celeron_20conv_30bs.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gianpaolo/PycharmProjects/Aca2018/resources/logs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gianpaolo/PycharmProjects/Aca2018/resources/logs/20conv_30bs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9382A3B2-9E32-D145-A845-58CCCA4757B5}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{918876C3-18C2-7B40-8414-F622F5DD02A0}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="440" windowWidth="33600" windowHeight="19260" tabRatio="991" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="i7_20conv_30bs" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179017" iterateDelta="1E-4"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
@@ -175,45 +175,55 @@
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
-  <c:style val="2"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
         <c:rich>
-          <a:bodyPr rot="0"/>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" strike="noStrike" spc="-1">
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
                 <a:solidFill>
-                  <a:srgbClr val="595959"/>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="95000"/>
+                  </a:schemeClr>
                 </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Calibri"/>
+                <a:effectLst>
+                  <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                    <a:prstClr val="black">
+                      <a:alpha val="40000"/>
+                    </a:prstClr>
+                  </a:outerShdw>
+                </a:effectLst>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="it-IT" sz="1400" b="0" strike="noStrike" spc="-1">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Calibri"/>
-              </a:rPr>
-              <a:t>Forward inference for different number of convolutions on Inter Xeon Platinum 8168</a:t>
+              <a:rPr lang="it-IT"/>
+              <a:t>Forward inference for different number of convolutions on Intel Celeron 877</a:t>
             </a:r>
           </a:p>
         </c:rich>
       </c:tx>
       <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -236,12 +246,19 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28440">
+            <a:ln w="34925" cap="rnd">
               <a:solidFill>
-                <a:srgbClr val="4472C4"/>
+                <a:schemeClr val="accent1"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
           </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
@@ -254,6 +271,27 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="it-IT"/>
+              </a:p>
+            </c:txPr>
             <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
@@ -359,12 +397,19 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28440">
+            <a:ln w="34925" cap="rnd">
               <a:solidFill>
-                <a:srgbClr val="ED7D31"/>
+                <a:schemeClr val="accent2"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
           </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
@@ -377,6 +422,27 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="it-IT"/>
+              </a:p>
+            </c:txPr>
             <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
@@ -477,9 +543,16 @@
         </c:dLbls>
         <c:hiLowLines>
           <c:spPr>
-            <a:ln>
-              <a:noFill/>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="54000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:prstDash val="dash"/>
             </a:ln>
+            <a:effectLst/>
           </c:spPr>
         </c:hiLowLines>
         <c:smooth val="0"/>
@@ -496,68 +569,68 @@
         <c:title>
           <c:tx>
             <c:rich>
-              <a:bodyPr rot="0"/>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
                     <a:solidFill>
-                      <a:srgbClr val="595959"/>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
                     </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="FFFFFF"/>
-                      </a:solidFill>
-                    </a:uFill>
-                    <a:latin typeface="Calibri"/>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="it-IT" sz="1000" b="0" strike="noStrike" spc="-1">
-                    <a:solidFill>
-                      <a:srgbClr val="595959"/>
-                    </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="FFFFFF"/>
-                      </a:solidFill>
-                    </a:uFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:rPr>
+                  <a:rPr lang="it-IT" cap="none" baseline="0"/>
                   <a:t>Number of convolution layers</a:t>
                 </a:r>
               </a:p>
             </c:rich>
           </c:tx>
           <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
-          <a:ln w="9360">
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:srgbClr val="D9D9D9"/>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="95000"/>
+                <a:alpha val="10000"/>
+              </a:schemeClr>
             </a:solidFill>
             <a:round/>
           </a:ln>
+          <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr/>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:srgbClr val="595959"/>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
                 </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Calibri"/>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="it-IT"/>
@@ -579,76 +652,77 @@
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
-            <a:ln w="9360">
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:srgbClr val="D9D9D9"/>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
+                </a:schemeClr>
               </a:solidFill>
               <a:round/>
             </a:ln>
+            <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
         <c:title>
           <c:tx>
             <c:rich>
-              <a:bodyPr rot="-5400000"/>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
                     <a:solidFill>
-                      <a:srgbClr val="595959"/>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
                     </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="FFFFFF"/>
-                      </a:solidFill>
-                    </a:uFill>
-                    <a:latin typeface="Calibri"/>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="it-IT" sz="1000" b="0" strike="noStrike" spc="-1">
-                    <a:solidFill>
-                      <a:srgbClr val="595959"/>
-                    </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="FFFFFF"/>
-                      </a:solidFill>
-                    </a:uFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:rPr>
+                  <a:rPr lang="it-IT" cap="none" baseline="0"/>
                   <a:t>Forward inference time [s]</a:t>
                 </a:r>
               </a:p>
             </c:rich>
           </c:tx>
           <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
-          <a:ln w="6480">
+          <a:noFill/>
+          <a:ln>
             <a:noFill/>
           </a:ln>
+          <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr/>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:srgbClr val="595959"/>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
                 </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Calibri"/>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="it-IT"/>
@@ -660,9 +734,10 @@
       </c:valAx>
       <c:spPr>
         <a:noFill/>
-        <a:ln w="25560">
+        <a:ln>
           <a:noFill/>
         </a:ln>
+        <a:effectLst/>
       </c:spPr>
     </c:plotArea>
     <c:legend>
@@ -673,23 +748,68 @@
         <a:ln>
           <a:noFill/>
         </a:ln>
+        <a:effectLst/>
       </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="it-IT"/>
+        </a:p>
+      </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="1"/>
   </c:chart>
   <c:spPr>
-    <a:solidFill>
-      <a:srgbClr val="FFFFFF"/>
-    </a:solidFill>
-    <a:ln w="9360">
-      <a:solidFill>
-        <a:srgbClr val="D9D9D9"/>
-      </a:solidFill>
-      <a:round/>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
     </a:ln>
+    <a:effectLst/>
   </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="it-IT"/>
+    </a:p>
+  </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
@@ -703,66 +823,55 @@
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
-  <c:style val="2"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
         <c:rich>
-          <a:bodyPr rot="0"/>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" strike="noStrike" spc="-1">
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
                 <a:solidFill>
-                  <a:srgbClr val="595959"/>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="95000"/>
+                  </a:schemeClr>
                 </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Calibri"/>
+                <a:effectLst>
+                  <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                    <a:prstClr val="black">
+                      <a:alpha val="40000"/>
+                    </a:prstClr>
+                  </a:outerShdw>
+                </a:effectLst>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="it-IT" sz="1400" b="0" strike="noStrike" spc="-1">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Calibri"/>
-              </a:rPr>
-              <a:t>Network setup time for different number of convolutions on Intel </a:t>
+              <a:rPr lang="it-IT"/>
+              <a:t>Network setup time for different number of convolutions on Intel Celeron 877 </a:t>
             </a:r>
-            <a:r>
-              <a:rPr lang="it-IT" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                <a:effectLst/>
-              </a:rPr>
-              <a:t>Xeon Platinum 8168</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="it-IT" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0"/>
-              <a:t> </a:t>
-            </a:r>
-            <a:endParaRPr lang="it-IT" sz="1400" b="0" strike="noStrike" spc="-1">
-              <a:solidFill>
-                <a:srgbClr val="595959"/>
-              </a:solidFill>
-              <a:uFill>
-                <a:solidFill>
-                  <a:srgbClr val="FFFFFF"/>
-                </a:solidFill>
-              </a:uFill>
-              <a:latin typeface="Calibri"/>
-            </a:endParaRPr>
           </a:p>
         </c:rich>
       </c:tx>
       <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -785,12 +894,19 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28440">
+            <a:ln w="34925" cap="rnd">
               <a:solidFill>
-                <a:srgbClr val="4472C4"/>
+                <a:schemeClr val="accent1"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
           </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
@@ -803,6 +919,27 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="it-IT"/>
+              </a:p>
+            </c:txPr>
             <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
@@ -908,12 +1045,19 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28440">
+            <a:ln w="34925" cap="rnd">
               <a:solidFill>
-                <a:srgbClr val="ED7D31"/>
+                <a:schemeClr val="accent2"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
           </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
@@ -926,6 +1070,27 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="it-IT"/>
+              </a:p>
+            </c:txPr>
             <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
@@ -1026,9 +1191,16 @@
         </c:dLbls>
         <c:hiLowLines>
           <c:spPr>
-            <a:ln>
-              <a:noFill/>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="54000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:prstDash val="dash"/>
             </a:ln>
+            <a:effectLst/>
           </c:spPr>
         </c:hiLowLines>
         <c:smooth val="0"/>
@@ -1045,68 +1217,68 @@
         <c:title>
           <c:tx>
             <c:rich>
-              <a:bodyPr rot="0"/>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
                     <a:solidFill>
-                      <a:srgbClr val="595959"/>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
                     </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="FFFFFF"/>
-                      </a:solidFill>
-                    </a:uFill>
-                    <a:latin typeface="Calibri"/>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="it-IT" sz="1000" b="0" strike="noStrike" spc="-1">
-                    <a:solidFill>
-                      <a:srgbClr val="595959"/>
-                    </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="FFFFFF"/>
-                      </a:solidFill>
-                    </a:uFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:rPr>
+                  <a:rPr lang="it-IT" cap="none" baseline="0"/>
                   <a:t>Number of convolution layers</a:t>
                 </a:r>
               </a:p>
             </c:rich>
           </c:tx>
           <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
-          <a:ln w="9360">
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:srgbClr val="D9D9D9"/>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="95000"/>
+                <a:alpha val="10000"/>
+              </a:schemeClr>
             </a:solidFill>
             <a:round/>
           </a:ln>
+          <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr/>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:srgbClr val="595959"/>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
                 </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Calibri"/>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="it-IT"/>
@@ -1128,76 +1300,77 @@
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
-            <a:ln w="9360">
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:srgbClr val="D9D9D9"/>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
+                </a:schemeClr>
               </a:solidFill>
               <a:round/>
             </a:ln>
+            <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
         <c:title>
           <c:tx>
             <c:rich>
-              <a:bodyPr rot="-5400000"/>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
                     <a:solidFill>
-                      <a:srgbClr val="595959"/>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
                     </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="FFFFFF"/>
-                      </a:solidFill>
-                    </a:uFill>
-                    <a:latin typeface="Calibri"/>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="it-IT" sz="1000" b="0" strike="noStrike" spc="-1">
-                    <a:solidFill>
-                      <a:srgbClr val="595959"/>
-                    </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="FFFFFF"/>
-                      </a:solidFill>
-                    </a:uFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:rPr>
+                  <a:rPr lang="it-IT" cap="none" baseline="0"/>
                   <a:t>Setup time [ms]</a:t>
                 </a:r>
               </a:p>
             </c:rich>
           </c:tx>
           <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
-          <a:ln w="6480">
+          <a:noFill/>
+          <a:ln>
             <a:noFill/>
           </a:ln>
+          <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr/>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:srgbClr val="595959"/>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
                 </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Calibri"/>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="it-IT"/>
@@ -1209,9 +1382,10 @@
       </c:valAx>
       <c:spPr>
         <a:noFill/>
-        <a:ln w="25560">
+        <a:ln>
           <a:noFill/>
         </a:ln>
+        <a:effectLst/>
       </c:spPr>
     </c:plotArea>
     <c:legend>
@@ -1222,23 +1396,68 @@
         <a:ln>
           <a:noFill/>
         </a:ln>
+        <a:effectLst/>
       </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="it-IT"/>
+        </a:p>
+      </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="1"/>
   </c:chart>
   <c:spPr>
-    <a:solidFill>
-      <a:srgbClr val="FFFFFF"/>
-    </a:solidFill>
-    <a:ln w="9360">
-      <a:solidFill>
-        <a:srgbClr val="D9D9D9"/>
-      </a:solidFill>
-      <a:round/>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
     </a:ln>
+    <a:effectLst/>
   </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="it-IT"/>
+    </a:p>
+  </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
@@ -1252,66 +1471,55 @@
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
-  <c:style val="2"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
         <c:rich>
-          <a:bodyPr rot="0"/>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" strike="noStrike" spc="-1">
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
                 <a:solidFill>
-                  <a:srgbClr val="595959"/>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="95000"/>
+                  </a:schemeClr>
                 </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Calibri"/>
+                <a:effectLst>
+                  <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                    <a:prstClr val="black">
+                      <a:alpha val="40000"/>
+                    </a:prstClr>
+                  </a:outerShdw>
+                </a:effectLst>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="it-IT" sz="1400" b="0" strike="noStrike" spc="-1">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Calibri"/>
-              </a:rPr>
-              <a:t>Parameter memory usage for different number of convolutions on Intel </a:t>
+              <a:rPr lang="it-IT"/>
+              <a:t>Parameter memory usage for different number of convolutions on Intel Celeron 877 </a:t>
             </a:r>
-            <a:r>
-              <a:rPr lang="it-IT" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                <a:effectLst/>
-              </a:rPr>
-              <a:t>Xeon Platinum 8168</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="it-IT" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0"/>
-              <a:t> </a:t>
-            </a:r>
-            <a:endParaRPr lang="it-IT" sz="1400" b="0" strike="noStrike" spc="-1">
-              <a:solidFill>
-                <a:srgbClr val="595959"/>
-              </a:solidFill>
-              <a:uFill>
-                <a:solidFill>
-                  <a:srgbClr val="FFFFFF"/>
-                </a:solidFill>
-              </a:uFill>
-              <a:latin typeface="Calibri"/>
-            </a:endParaRPr>
           </a:p>
         </c:rich>
       </c:tx>
       <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -1334,12 +1542,19 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28440">
+            <a:ln w="34925" cap="rnd">
               <a:solidFill>
-                <a:srgbClr val="4472C4"/>
+                <a:schemeClr val="accent1"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
           </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
@@ -1352,6 +1567,27 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="it-IT"/>
+              </a:p>
+            </c:txPr>
             <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
@@ -1457,12 +1693,19 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28440">
+            <a:ln w="34925" cap="rnd">
               <a:solidFill>
-                <a:srgbClr val="ED7D31"/>
+                <a:schemeClr val="accent2"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
           </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
@@ -1475,6 +1718,27 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="it-IT"/>
+              </a:p>
+            </c:txPr>
             <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
@@ -1575,9 +1839,16 @@
         </c:dLbls>
         <c:hiLowLines>
           <c:spPr>
-            <a:ln>
-              <a:noFill/>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="54000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:prstDash val="dash"/>
             </a:ln>
+            <a:effectLst/>
           </c:spPr>
         </c:hiLowLines>
         <c:smooth val="0"/>
@@ -1594,68 +1865,68 @@
         <c:title>
           <c:tx>
             <c:rich>
-              <a:bodyPr rot="0"/>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
                     <a:solidFill>
-                      <a:srgbClr val="595959"/>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
                     </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="FFFFFF"/>
-                      </a:solidFill>
-                    </a:uFill>
-                    <a:latin typeface="Calibri"/>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="it-IT" sz="1000" b="0" strike="noStrike" spc="-1">
-                    <a:solidFill>
-                      <a:srgbClr val="595959"/>
-                    </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="FFFFFF"/>
-                      </a:solidFill>
-                    </a:uFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:rPr>
+                  <a:rPr lang="it-IT" cap="none" baseline="0"/>
                   <a:t>Numeber of convolution layers</a:t>
                 </a:r>
               </a:p>
             </c:rich>
           </c:tx>
           <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
-          <a:ln w="9360">
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:srgbClr val="D9D9D9"/>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="95000"/>
+                <a:alpha val="10000"/>
+              </a:schemeClr>
             </a:solidFill>
             <a:round/>
           </a:ln>
+          <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr/>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:srgbClr val="595959"/>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
                 </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Calibri"/>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="it-IT"/>
@@ -1677,76 +1948,77 @@
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
-            <a:ln w="9360">
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:srgbClr val="D9D9D9"/>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
+                </a:schemeClr>
               </a:solidFill>
               <a:round/>
             </a:ln>
+            <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
         <c:title>
           <c:tx>
             <c:rich>
-              <a:bodyPr rot="-5400000"/>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
                     <a:solidFill>
-                      <a:srgbClr val="595959"/>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
                     </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="FFFFFF"/>
-                      </a:solidFill>
-                    </a:uFill>
-                    <a:latin typeface="Calibri"/>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="it-IT" sz="1000" b="0" strike="noStrike" spc="-1">
-                    <a:solidFill>
-                      <a:srgbClr val="595959"/>
-                    </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="FFFFFF"/>
-                      </a:solidFill>
-                    </a:uFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:rPr>
+                  <a:rPr lang="it-IT" cap="none" baseline="0"/>
                   <a:t>Memory usage [kB]</a:t>
                 </a:r>
               </a:p>
             </c:rich>
           </c:tx>
           <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
-          <a:ln w="6480">
+          <a:noFill/>
+          <a:ln>
             <a:noFill/>
           </a:ln>
+          <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr/>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:srgbClr val="595959"/>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
                 </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Calibri"/>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="it-IT"/>
@@ -1758,9 +2030,10 @@
       </c:valAx>
       <c:spPr>
         <a:noFill/>
-        <a:ln w="25560">
+        <a:ln>
           <a:noFill/>
         </a:ln>
+        <a:effectLst/>
       </c:spPr>
     </c:plotArea>
     <c:legend>
@@ -1771,23 +2044,68 @@
         <a:ln>
           <a:noFill/>
         </a:ln>
+        <a:effectLst/>
       </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="it-IT"/>
+        </a:p>
+      </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="1"/>
   </c:chart>
   <c:spPr>
-    <a:solidFill>
-      <a:srgbClr val="FFFFFF"/>
-    </a:solidFill>
-    <a:ln w="9360">
-      <a:solidFill>
-        <a:srgbClr val="D9D9D9"/>
-      </a:solidFill>
-      <a:round/>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
     </a:ln>
+    <a:effectLst/>
   </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="it-IT"/>
+    </a:p>
+  </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
@@ -1801,66 +2119,63 @@
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
-  <c:style val="2"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
         <c:rich>
-          <a:bodyPr rot="0"/>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" strike="noStrike" spc="-1">
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
                 <a:solidFill>
-                  <a:srgbClr val="595959"/>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="95000"/>
+                  </a:schemeClr>
                 </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Calibri"/>
+                <a:effectLst>
+                  <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                    <a:prstClr val="black">
+                      <a:alpha val="40000"/>
+                    </a:prstClr>
+                  </a:outerShdw>
+                </a:effectLst>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="it-IT" sz="1400" b="0" strike="noStrike" spc="-1">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Calibri"/>
-              </a:rPr>
-              <a:t>Inner buffers memory usage for different convolutions on Intel </a:t>
+              <a:rPr lang="it-IT"/>
+              <a:t>Inner buffers memory usage for different convolutions on</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="it-IT" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                <a:effectLst/>
-              </a:rPr>
-              <a:t>Xeon Platinum 8168</a:t>
+              <a:rPr lang="it-IT" baseline="0"/>
+              <a:t> </a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="it-IT" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0"/>
-              <a:t> </a:t>
+              <a:rPr lang="it-IT"/>
+              <a:t>Intel Celeron 877 </a:t>
             </a:r>
-            <a:endParaRPr lang="it-IT" sz="1400" b="0" strike="noStrike" spc="-1">
-              <a:solidFill>
-                <a:srgbClr val="595959"/>
-              </a:solidFill>
-              <a:uFill>
-                <a:solidFill>
-                  <a:srgbClr val="FFFFFF"/>
-                </a:solidFill>
-              </a:uFill>
-              <a:latin typeface="Calibri"/>
-            </a:endParaRPr>
           </a:p>
         </c:rich>
       </c:tx>
       <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -1883,12 +2198,19 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28440">
+            <a:ln w="34925" cap="rnd">
               <a:solidFill>
-                <a:srgbClr val="4472C4"/>
+                <a:schemeClr val="accent1"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
           </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
@@ -1901,6 +2223,27 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="it-IT"/>
+              </a:p>
+            </c:txPr>
             <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
@@ -2006,12 +2349,19 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28440">
+            <a:ln w="34925" cap="rnd">
               <a:solidFill>
-                <a:srgbClr val="ED7D31"/>
+                <a:schemeClr val="accent2"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
           </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
@@ -2024,6 +2374,27 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="it-IT"/>
+              </a:p>
+            </c:txPr>
             <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
@@ -2124,9 +2495,16 @@
         </c:dLbls>
         <c:hiLowLines>
           <c:spPr>
-            <a:ln>
-              <a:noFill/>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="54000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:prstDash val="dash"/>
             </a:ln>
+            <a:effectLst/>
           </c:spPr>
         </c:hiLowLines>
         <c:smooth val="0"/>
@@ -2143,68 +2521,68 @@
         <c:title>
           <c:tx>
             <c:rich>
-              <a:bodyPr rot="0"/>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
                     <a:solidFill>
-                      <a:srgbClr val="595959"/>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
                     </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="FFFFFF"/>
-                      </a:solidFill>
-                    </a:uFill>
-                    <a:latin typeface="Calibri"/>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="it-IT" sz="1000" b="0" strike="noStrike" spc="-1">
-                    <a:solidFill>
-                      <a:srgbClr val="595959"/>
-                    </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="FFFFFF"/>
-                      </a:solidFill>
-                    </a:uFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:rPr>
+                  <a:rPr lang="it-IT" cap="none" baseline="0"/>
                   <a:t>Number of convolution layers</a:t>
                 </a:r>
               </a:p>
             </c:rich>
           </c:tx>
           <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
-          <a:ln w="9360">
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:srgbClr val="D9D9D9"/>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="95000"/>
+                <a:alpha val="10000"/>
+              </a:schemeClr>
             </a:solidFill>
             <a:round/>
           </a:ln>
+          <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr/>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:srgbClr val="595959"/>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
                 </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Calibri"/>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="it-IT"/>
@@ -2226,76 +2604,77 @@
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
-            <a:ln w="9360">
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:srgbClr val="D9D9D9"/>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
+                </a:schemeClr>
               </a:solidFill>
               <a:round/>
             </a:ln>
+            <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
         <c:title>
           <c:tx>
             <c:rich>
-              <a:bodyPr rot="-5400000"/>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
                     <a:solidFill>
-                      <a:srgbClr val="595959"/>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
                     </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="FFFFFF"/>
-                      </a:solidFill>
-                    </a:uFill>
-                    <a:latin typeface="Calibri"/>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="it-IT" sz="1000" b="0" strike="noStrike" spc="-1">
-                    <a:solidFill>
-                      <a:srgbClr val="595959"/>
-                    </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="FFFFFF"/>
-                      </a:solidFill>
-                    </a:uFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:rPr>
+                  <a:rPr lang="it-IT" cap="none" baseline="0"/>
                   <a:t>Memory usage [MB]</a:t>
                 </a:r>
               </a:p>
             </c:rich>
           </c:tx>
           <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
-          <a:ln w="6480">
+          <a:noFill/>
+          <a:ln>
             <a:noFill/>
           </a:ln>
+          <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr/>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:srgbClr val="595959"/>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
                 </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Calibri"/>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="it-IT"/>
@@ -2307,9 +2686,10 @@
       </c:valAx>
       <c:spPr>
         <a:noFill/>
-        <a:ln w="25560">
+        <a:ln>
           <a:noFill/>
         </a:ln>
+        <a:effectLst/>
       </c:spPr>
     </c:plotArea>
     <c:legend>
@@ -2320,23 +2700,68 @@
         <a:ln>
           <a:noFill/>
         </a:ln>
+        <a:effectLst/>
       </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="it-IT"/>
+        </a:p>
+      </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="1"/>
   </c:chart>
   <c:spPr>
-    <a:solidFill>
-      <a:srgbClr val="FFFFFF"/>
-    </a:solidFill>
-    <a:ln w="9360">
-      <a:solidFill>
-        <a:srgbClr val="D9D9D9"/>
-      </a:solidFill>
-      <a:round/>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
     </a:ln>
+    <a:effectLst/>
   </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="it-IT"/>
+    </a:p>
+  </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
@@ -2793,8 +3218,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="168" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView tabSelected="1" topLeftCell="P1" zoomScale="168" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AB7" sqref="AB7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>

</xml_diff>